<commit_message>
Number of words reduced by 745!
</commit_message>
<xml_diff>
--- a/WordCount.xlsx
+++ b/WordCount.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="338" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="169" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,18 +15,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+  <si>
+    <t>Words</t>
+  </si>
+  <si>
+    <t>Figs/Tab/Eqn</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
   <si>
     <t>Para #</t>
   </si>
   <si>
-    <t>Words</t>
-  </si>
-  <si>
     <t>Figure caption #</t>
   </si>
   <si>
     <t>Table caption #</t>
+  </si>
+  <si>
+    <t>Figures</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>Equations</t>
   </si>
 </sst>
 </file>
@@ -36,11 +51,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -56,6 +72,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -100,8 +123,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -120,52 +147,73 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.52551020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.1377551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="0" t="n">
         <f aca="false">SUM(B3:B44) + SUM(E3:E6) + E10</f>
-        <v>3206</v>
+        <v>2472</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="0" t="n">
+        <f aca="false">SUM(E13:E19)</f>
+        <v>1033</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="0" t="n">
+        <f aca="false">B1+D1</f>
+        <v>3505</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>1</v>
-      </c>
       <c r="D2" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="0" t="n">
-        <v>90</v>
+      <c r="B3" s="1" t="n">
+        <v>80</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E3" s="0" t="n">
-        <v>129</v>
+      <c r="E3" s="1" t="n">
+        <v>111</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -173,14 +221,14 @@
         <f aca="false">A3+1</f>
         <v>2</v>
       </c>
-      <c r="B4" s="0" t="n">
-        <v>80</v>
+      <c r="B4" s="1" t="n">
+        <v>77</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E4" s="0" t="n">
-        <v>110</v>
+      <c r="E4" s="1" t="n">
+        <v>105</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -188,14 +236,14 @@
         <f aca="false">A4+1</f>
         <v>3</v>
       </c>
-      <c r="B5" s="0" t="n">
-        <v>137</v>
+      <c r="B5" s="1" t="n">
+        <v>127</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="E5" s="0" t="n">
-        <v>69</v>
+      <c r="E5" s="1" t="n">
+        <v>46</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -203,14 +251,14 @@
         <f aca="false">A5+1</f>
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="n">
-        <v>95</v>
+      <c r="B6" s="1" t="n">
+        <v>86</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="E6" s="0" t="n">
-        <v>158</v>
+      <c r="E6" s="1" t="n">
+        <v>75</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -218,8 +266,8 @@
         <f aca="false">A6+1</f>
         <v>5</v>
       </c>
-      <c r="B7" s="0" t="n">
-        <v>28</v>
+      <c r="B7" s="1" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -227,8 +275,8 @@
         <f aca="false">A7+1</f>
         <v>6</v>
       </c>
-      <c r="B8" s="0" t="n">
-        <v>158</v>
+      <c r="B8" s="1" t="n">
+        <v>138</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -236,14 +284,14 @@
         <f aca="false">A8+1</f>
         <v>7</v>
       </c>
-      <c r="B9" s="0" t="n">
-        <v>32</v>
+      <c r="B9" s="1" t="n">
+        <v>19</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -251,8 +299,8 @@
         <f aca="false">A9+1</f>
         <v>8</v>
       </c>
-      <c r="B10" s="0" t="n">
-        <v>377</v>
+      <c r="B10" s="1" t="n">
+        <v>298</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>1</v>
@@ -266,8 +314,8 @@
         <f aca="false">A10+1</f>
         <v>9</v>
       </c>
-      <c r="B11" s="0" t="n">
-        <v>28</v>
+      <c r="B11" s="1" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -275,8 +323,11 @@
         <f aca="false">A11+1</f>
         <v>10</v>
       </c>
-      <c r="B12" s="0" t="n">
-        <v>124</v>
+      <c r="B12" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -284,8 +335,14 @@
         <f aca="false">A12+1</f>
         <v>11</v>
       </c>
-      <c r="B13" s="0" t="n">
-        <v>43</v>
+      <c r="B13" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>122</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -293,8 +350,14 @@
         <f aca="false">A13+1</f>
         <v>12</v>
       </c>
-      <c r="B14" s="0" t="n">
-        <v>167</v>
+      <c r="B14" s="1" t="n">
+        <v>159</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>186</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -302,8 +365,14 @@
         <f aca="false">A14+1</f>
         <v>13</v>
       </c>
-      <c r="B15" s="0" t="n">
-        <v>86</v>
+      <c r="B15" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>311</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -311,8 +380,14 @@
         <f aca="false">A15+1</f>
         <v>14</v>
       </c>
-      <c r="B16" s="0" t="n">
-        <v>167</v>
+      <c r="B16" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>114</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -320,8 +395,8 @@
         <f aca="false">A16+1</f>
         <v>15</v>
       </c>
-      <c r="B17" s="0" t="n">
-        <v>144</v>
+      <c r="B17" s="1" t="n">
+        <v>116</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -329,8 +404,14 @@
         <f aca="false">A17+1</f>
         <v>16</v>
       </c>
-      <c r="B18" s="0" t="n">
-        <v>105</v>
+      <c r="B18" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>156</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -338,8 +419,14 @@
         <f aca="false">A18+1</f>
         <v>17</v>
       </c>
-      <c r="B19" s="0" t="n">
-        <v>64</v>
+      <c r="B19" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>144</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -347,8 +434,8 @@
         <f aca="false">A19+1</f>
         <v>18</v>
       </c>
-      <c r="B20" s="0" t="n">
-        <v>86</v>
+      <c r="B20" s="1" t="n">
+        <v>54</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -356,8 +443,8 @@
         <f aca="false">A20+1</f>
         <v>19</v>
       </c>
-      <c r="B21" s="0" t="n">
-        <v>142</v>
+      <c r="B21" s="1" t="n">
+        <v>122</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -365,8 +452,8 @@
         <f aca="false">A21+1</f>
         <v>20</v>
       </c>
-      <c r="B22" s="0" t="n">
-        <v>144</v>
+      <c r="B22" s="1" t="n">
+        <v>96</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -374,8 +461,8 @@
         <f aca="false">A22+1</f>
         <v>21</v>
       </c>
-      <c r="B23" s="0" t="n">
-        <v>174</v>
+      <c r="B23" s="1" t="n">
+        <v>110</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -384,7 +471,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>106</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -392,122 +479,8 @@
         <f aca="false">A24+1</f>
         <v>23</v>
       </c>
-      <c r="B25" s="0" t="n">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
-        <f aca="false">A25+1</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
-        <f aca="false">A26+1</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="n">
-        <f aca="false">A27+1</f>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
-        <f aca="false">A28+1</f>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="n">
-        <f aca="false">A29+1</f>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
-        <f aca="false">A30+1</f>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="n">
-        <f aca="false">A31+1</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="n">
-        <f aca="false">A32+1</f>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="n">
-        <f aca="false">A33+1</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="n">
-        <f aca="false">A34+1</f>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="n">
-        <f aca="false">A35+1</f>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="n">
-        <f aca="false">A36+1</f>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="n">
-        <f aca="false">A37+1</f>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="n">
-        <f aca="false">A38+1</f>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="n">
-        <f aca="false">A39+1</f>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="n">
-        <f aca="false">A40+1</f>
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="n">
-        <f aca="false">A41+1</f>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="n">
-        <f aca="false">A42+1</f>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="n">
-        <f aca="false">A43+1</f>
-        <v>42</v>
+      <c r="B25" s="1" t="n">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Word count from Ravi's figure updated
</commit_message>
<xml_diff>
--- a/WordCount.xlsx
+++ b/WordCount.xlsx
@@ -153,7 +153,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
@@ -178,14 +178,14 @@
       </c>
       <c r="D1" s="0" t="n">
         <f aca="false">SUM(E13:E19)</f>
-        <v>1033</v>
+        <v>1008</v>
       </c>
       <c r="F1" s="0" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="0" t="n">
         <f aca="false">B1+D1</f>
-        <v>3505</v>
+        <v>3480</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -372,7 +372,8 @@
         <v>3</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>311</v>
+        <f aca="false">ROUND(300/0.5/2.44+40)</f>
+        <v>286</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>